<commit_message>
Committing code with changes for Extend Nav to JDE
</commit_message>
<xml_diff>
--- a/Mendix/input/data/Local_Vendor_Data.xlsx
+++ b/Mendix/input/data/Local_Vendor_Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Documents\Heniken\Latest 25.2.19\Mendix\input\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CC4E21D-2F63-4AE8-9EA9-DD7A42217CFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13320" windowHeight="2436"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13320" windowHeight="2436" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestPlan" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="90">
   <si>
     <t>S.NO</t>
   </si>
@@ -219,13 +220,85 @@
   </si>
   <si>
     <t>Extend Vendor Global and local with Rejections for NAV (For Algeria to panama)</t>
+  </si>
+  <si>
+    <t>A/B Amount Currency</t>
+  </si>
+  <si>
+    <t>Payment Terms</t>
+  </si>
+  <si>
+    <t>Text Rate Area</t>
+  </si>
+  <si>
+    <t>Payment creation</t>
+  </si>
+  <si>
+    <t>Hold Payment</t>
+  </si>
+  <si>
+    <t>GL Class</t>
+  </si>
+  <si>
+    <t>Tax EPL Code</t>
+  </si>
+  <si>
+    <t>Payment Metods</t>
+  </si>
+  <si>
+    <t>PQ, P*Q Contracts</t>
+  </si>
+  <si>
+    <t>Send Method</t>
+  </si>
+  <si>
+    <t>3, Email</t>
+  </si>
+  <si>
+    <t>Default Currency</t>
+  </si>
+  <si>
+    <t>Bank Bearer</t>
+  </si>
+  <si>
+    <t>V002, Payment within 7 days</t>
+  </si>
+  <si>
+    <t>SGGST100, Tax rate/Area</t>
+  </si>
+  <si>
+    <t>Y, By Pay Items</t>
+  </si>
+  <si>
+    <t>2, Hold payment, allow voucher</t>
+  </si>
+  <si>
+    <t>P001, A/P Trade 3 Party Supplier</t>
+  </si>
+  <si>
+    <t>SGD, Singapore Dollar</t>
+  </si>
+  <si>
+    <t>VE, VAT - Exempt Supplies</t>
+  </si>
+  <si>
+    <t>C, Cheque</t>
+  </si>
+  <si>
+    <t>001, Heineken bears the cost</t>
+  </si>
+  <si>
+    <t>SG04</t>
+  </si>
+  <si>
+    <t>69Extend Vendor Global and Local from  SAP to JDE (With Local data adding)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Mic Shell Dlg"/>
@@ -240,8 +313,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,40 +329,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -312,19 +373,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,37 +721,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:IY2"/>
+  <dimension ref="A1:IY3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="6.33203125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="44.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.5546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="14" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.33203125" style="4" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.6640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11" style="4" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.44140625" style="4" customWidth="1" collapsed="1"/>
-    <col min="16" max="257" width="9.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="258" max="258" width="9.109375" style="6" collapsed="1"/>
-    <col min="259" max="259" width="9.109375" style="6"/>
-    <col min="260" max="16384" width="9.109375" style="6" collapsed="1"/>
+    <col min="1" max="1" width="5.44140625" style="6" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="6.33203125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="76.109375" style="6" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.88671875" style="6" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.44140625" style="6" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.6640625" style="6" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.44140625" style="6" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="24.77734375" style="6" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20" style="6" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="23.88671875" style="6" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.6640625" style="6" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="21.109375" style="6" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="26.33203125" style="6" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="30.109375" style="6" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="26.109375" style="6" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="31.44140625" style="6" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.88671875" style="6" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="19.77734375" style="6" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="26.77734375" style="6" customWidth="1" collapsed="1"/>
+    <col min="20" max="257" width="9.109375" style="6" customWidth="1" collapsed="1"/>
+    <col min="258" max="258" width="9.109375" style="7" collapsed="1"/>
+    <col min="259" max="259" width="9.109375" style="7"/>
+    <col min="260" max="16384" width="9.109375" style="7" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -705,60 +769,169 @@
       <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-    </row>
-    <row r="2" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="I1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G3" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
+      <c r="I3" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -771,7 +944,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:IV6"/>
   <sheetViews>
@@ -904,7 +1077,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:IV21"/>
   <sheetViews>

</xml_diff>